<commit_message>
add functionality to lookup table: a separate worksheet for variable type (stock or flow) and its label
</commit_message>
<xml_diff>
--- a/misc/lookup.xlsx
+++ b/misc/lookup.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asacarny/Research/Public Files/cost reports/misc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asacarny/Repositories/hospital-cost-reports/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{45971BC6-0DF4-3642-BBB5-A74DB58BB2FB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B372BF-D429-C747-869F-F2702959EA83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16340" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="18640" windowHeight="16120" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Type and Label" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="112">
   <si>
     <t>rec</t>
   </si>
@@ -262,6 +263,105 @@
   </si>
   <si>
     <t>03100</t>
+  </si>
+  <si>
+    <t>beds - adults &amp; peds</t>
+  </si>
+  <si>
+    <t>bed days available in rpt period</t>
+  </si>
+  <si>
+    <t>inpatient bed days utilized</t>
+  </si>
+  <si>
+    <t>inpatient discharges</t>
+  </si>
+  <si>
+    <t>beds - total adults &amp; peds incl swing beds</t>
+  </si>
+  <si>
+    <t>beds - total (inc swing + spec care beds e.g. icu, ccu, nicu)</t>
+  </si>
+  <si>
+    <t>investment income</t>
+  </si>
+  <si>
+    <t>inpatient hospital revenue</t>
+  </si>
+  <si>
+    <t>inpatient general revenue (total of hosp, ipf, irf, snf, etc.)</t>
+  </si>
+  <si>
+    <t>inpatient intensive care type revenue (total of icu, ccu, etc.)</t>
+  </si>
+  <si>
+    <t>inpatient routine care revenue (sum of ipgenrev and ipicrev)</t>
+  </si>
+  <si>
+    <t>inpatient ancillary services revenue</t>
+  </si>
+  <si>
+    <t>inpatient outpatient services revenue</t>
+  </si>
+  <si>
+    <t>inpatient total patient revenue</t>
+  </si>
+  <si>
+    <t>outpatient ancillary services revenue</t>
+  </si>
+  <si>
+    <t>outpatient outpatient services revenue</t>
+  </si>
+  <si>
+    <t>outpatient total patient revenues</t>
+  </si>
+  <si>
+    <t>total patient revenue (sum of iptotrev and optotrev)</t>
+  </si>
+  <si>
+    <t>cost to charge ratio</t>
+  </si>
+  <si>
+    <t>other uncompensated care charges (1996 format only)</t>
+  </si>
+  <si>
+    <t>total initial obligation of patients for charity care (2010 format only)</t>
+  </si>
+  <si>
+    <t>partial payment by patients approved for charity care (2010 format only)</t>
+  </si>
+  <si>
+    <t>non-medicare &amp; non-reimbursable medicare bad debt expense (2010 format only)</t>
+  </si>
+  <si>
+    <t>cost of uncompensated care (2010 format only)</t>
+  </si>
+  <si>
+    <t>net patient revenues (total revenues minus allowances &amp; discounts)</t>
+  </si>
+  <si>
+    <t>other income</t>
+  </si>
+  <si>
+    <t>total operating expenses</t>
+  </si>
+  <si>
+    <t>total other expenses</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>dollar_flow</t>
+  </si>
+  <si>
+    <t>flow</t>
+  </si>
+  <si>
+    <t>stock</t>
   </si>
 </sst>
 </file>
@@ -614,18 +714,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2BB4DF-E65D-224C-B8BB-1875153B4956}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -644,8 +747,10 @@
       <c r="F1" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -664,8 +769,9 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -684,8 +790,9 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -704,8 +811,9 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -724,8 +832,9 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -744,8 +853,9 @@
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -764,8 +874,9 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -784,8 +895,9 @@
       <c r="F8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -804,8 +916,9 @@
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -824,8 +937,9 @@
       <c r="F10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -844,8 +958,9 @@
       <c r="F11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -864,8 +979,9 @@
       <c r="F12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -884,8 +1000,9 @@
       <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -904,8 +1021,9 @@
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -924,8 +1042,9 @@
       <c r="F15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -944,8 +1063,9 @@
       <c r="F16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -964,8 +1084,9 @@
       <c r="F17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -984,8 +1105,9 @@
       <c r="F18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1004,8 +1126,9 @@
       <c r="F19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
@@ -1024,8 +1147,9 @@
       <c r="F20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -1044,8 +1168,9 @@
       <c r="F21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -1064,8 +1189,9 @@
       <c r="F22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -1084,8 +1210,9 @@
       <c r="F23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -1104,8 +1231,9 @@
       <c r="F24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -1124,8 +1252,9 @@
       <c r="F25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -1144,8 +1273,9 @@
       <c r="F26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
@@ -1164,8 +1294,9 @@
       <c r="F27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
@@ -1184,8 +1315,9 @@
       <c r="F28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>54</v>
       </c>
@@ -1204,8 +1336,9 @@
       <c r="F29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
@@ -1225,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>68</v>
       </c>
@@ -1245,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>69</v>
       </c>
@@ -1265,7 +1398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>70</v>
       </c>
@@ -1285,7 +1418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
@@ -1305,7 +1438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
@@ -1324,8 +1457,9 @@
       <c r="F35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
@@ -1344,8 +1478,9 @@
       <c r="F36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>11</v>
       </c>
@@ -1364,8 +1499,9 @@
       <c r="F37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>13</v>
       </c>
@@ -1384,8 +1520,9 @@
       <c r="F38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>15</v>
       </c>
@@ -1404,8 +1541,9 @@
       <c r="F39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -1424,8 +1562,9 @@
       <c r="F40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>19</v>
       </c>
@@ -1444,8 +1583,9 @@
       <c r="F41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>21</v>
       </c>
@@ -1464,8 +1604,9 @@
       <c r="F42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>23</v>
       </c>
@@ -1484,8 +1625,9 @@
       <c r="F43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -1504,8 +1646,9 @@
       <c r="F44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>27</v>
       </c>
@@ -1524,8 +1667,9 @@
       <c r="F45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -1544,8 +1688,9 @@
       <c r="F46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>31</v>
       </c>
@@ -1564,8 +1709,9 @@
       <c r="F47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>32</v>
       </c>
@@ -1584,8 +1730,9 @@
       <c r="F48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>34</v>
       </c>
@@ -1604,8 +1751,9 @@
       <c r="F49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>35</v>
       </c>
@@ -1624,8 +1772,9 @@
       <c r="F50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>36</v>
       </c>
@@ -1644,8 +1793,9 @@
       <c r="F51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>37</v>
       </c>
@@ -1665,7 +1815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>61</v>
       </c>
@@ -1684,8 +1834,9 @@
       <c r="F53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>46</v>
       </c>
@@ -1705,7 +1856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>48</v>
       </c>
@@ -1724,8 +1875,9 @@
       <c r="F55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>49</v>
       </c>
@@ -1744,8 +1896,9 @@
       <c r="F56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>51</v>
       </c>
@@ -1764,8 +1917,9 @@
       <c r="F57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>53</v>
       </c>
@@ -1785,7 +1939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>54</v>
       </c>
@@ -1805,7 +1959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>77</v>
       </c>
@@ -1824,9 +1978,360 @@
       <c r="F60">
         <v>0</v>
       </c>
+      <c r="G60" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F01AFD1-3AE8-2C43-8863-F91A96C0A348}">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add variables for critical care beds
</commit_message>
<xml_diff>
--- a/misc/lookup.xlsx
+++ b/misc/lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asacarny/Repositories/hospital-cost-reports/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B372BF-D429-C747-869F-F2702959EA83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAD4803-78DF-894F-821E-D9EC0667DE3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="18640" windowHeight="16120" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
+    <workbookView xWindow="15760" yWindow="3720" windowWidth="18640" windowHeight="16120" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Table" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="124">
   <si>
     <t>rec</t>
   </si>
@@ -362,6 +362,42 @@
   </si>
   <si>
     <t>stock</t>
+  </si>
+  <si>
+    <t>icu_beds</t>
+  </si>
+  <si>
+    <t>ccu_beds</t>
+  </si>
+  <si>
+    <t>bicu_beds</t>
+  </si>
+  <si>
+    <t>sicu_beds</t>
+  </si>
+  <si>
+    <t>othspec_beds</t>
+  </si>
+  <si>
+    <t>01100</t>
+  </si>
+  <si>
+    <t>intensive care unit beds</t>
+  </si>
+  <si>
+    <t>coronary care unit beds</t>
+  </si>
+  <si>
+    <t>burn intensive care unit beds</t>
+  </si>
+  <si>
+    <t>surgical intensive care unit beds</t>
+  </si>
+  <si>
+    <t>other special care beds</t>
+  </si>
+  <si>
+    <t>02140</t>
   </si>
 </sst>
 </file>
@@ -714,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2BB4DF-E65D-224C-B8BB-1875153B4956}">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63:F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1319,7 +1355,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>47</v>
@@ -1328,7 +1364,7 @@
         <v>33</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E29">
         <v>10</v>
@@ -1340,212 +1376,212 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="E30">
         <v>10</v>
       </c>
       <c r="F30">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="E31">
         <v>10</v>
       </c>
       <c r="F31">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="E32">
         <v>10</v>
       </c>
       <c r="F32">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E33">
         <v>10</v>
       </c>
       <c r="F33">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="E34">
         <v>10</v>
       </c>
       <c r="F34">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="E35">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35" s="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="E36">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36" s="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="E37">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37" s="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="E38">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="F38">
-        <v>1</v>
-      </c>
-      <c r="G38" s="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="E39">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39" s="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>6</v>
@@ -1554,7 +1590,7 @@
         <v>56</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E40">
         <v>96</v>
@@ -1566,16 +1602,16 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E41">
         <v>96</v>
@@ -1587,16 +1623,16 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="E42">
         <v>96</v>
@@ -1608,16 +1644,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E43">
         <v>96</v>
@@ -1629,16 +1665,16 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E44">
         <v>96</v>
@@ -1650,16 +1686,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E45">
         <v>96</v>
@@ -1671,7 +1707,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>20</v>
@@ -1680,7 +1716,7 @@
         <v>56</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E46">
         <v>96</v>
@@ -1692,7 +1728,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>20</v>
@@ -1701,7 +1737,7 @@
         <v>56</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="E47">
         <v>96</v>
@@ -1713,16 +1749,16 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="E48">
         <v>96</v>
@@ -1734,16 +1770,16 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E49">
         <v>96</v>
@@ -1755,16 +1791,16 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E50">
         <v>96</v>
@@ -1776,16 +1812,16 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="E51">
         <v>96</v>
@@ -1797,16 +1833,16 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="E52">
         <v>96</v>
@@ -1814,19 +1850,20 @@
       <c r="F52">
         <v>1</v>
       </c>
+      <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E53">
         <v>96</v>
@@ -1838,16 +1875,16 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="E54">
         <v>96</v>
@@ -1855,19 +1892,20 @@
       <c r="F54">
         <v>1</v>
       </c>
+      <c r="G54" s="1"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E55">
         <v>96</v>
@@ -1879,16 +1917,16 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E56">
         <v>96</v>
@@ -1900,16 +1938,16 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="E57">
         <v>96</v>
@@ -1917,20 +1955,19 @@
       <c r="F57">
         <v>1</v>
       </c>
-      <c r="G57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="E58">
         <v>96</v>
@@ -1938,10 +1975,11 @@
       <c r="F58">
         <v>1</v>
       </c>
+      <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>47</v>
@@ -1950,7 +1988,7 @@
         <v>56</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="E59">
         <v>96</v>
@@ -1961,24 +1999,231 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60">
+        <v>96</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61">
+        <v>96</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62">
+        <v>96</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E63">
+        <v>96</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E64">
+        <v>96</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E65">
+        <v>96</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E66">
+        <v>96</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E67">
+        <v>96</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E68">
+        <v>96</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E69">
+        <v>96</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E60">
-        <v>96</v>
-      </c>
-      <c r="F60">
+      <c r="E70">
+        <v>96</v>
+      </c>
+      <c r="F70">
         <v>0</v>
       </c>
-      <c r="G60" s="1"/>
+      <c r="G70" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1988,10 +2233,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F01AFD1-3AE8-2C43-8863-F91A96C0A348}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2311,23 +2556,78 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C35" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected label for nonmcbaddebt field (thank you Ken Michelson for finding this bug) Added labels for disabled uncompensated care variables should they eventually be enabled.
</commit_message>
<xml_diff>
--- a/misc/lookup.xlsx
+++ b/misc/lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asacarny/Repositories/hospital-cost-reports/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAD4803-78DF-894F-821E-D9EC0667DE3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2128C3-4C94-A44A-BF78-E2141C1BC4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15760" yWindow="3720" windowWidth="18640" windowHeight="16120" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
+    <workbookView xWindow="15760" yWindow="3720" windowWidth="18640" windowHeight="16120" activeTab="1" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Table" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="129">
   <si>
     <t>rec</t>
   </si>
@@ -331,9 +331,6 @@
     <t>partial payment by patients approved for charity care (2010 format only)</t>
   </si>
   <si>
-    <t>non-medicare &amp; non-reimbursable medicare bad debt expense (2010 format only)</t>
-  </si>
-  <si>
     <t>cost of uncompensated care (2010 format only)</t>
   </si>
   <si>
@@ -398,6 +395,24 @@
   </si>
   <si>
     <t>02140</t>
+  </si>
+  <si>
+    <t>non-medicare bad debt expense (2010 format only)</t>
+  </si>
+  <si>
+    <t>medicare reimbursable bad debts (2010 format only)</t>
+  </si>
+  <si>
+    <t>cost of non-Medicare and non-reimbursable Medicare bad debt expense (2010 format only)</t>
+  </si>
+  <si>
+    <t>total bad debt expense (2010 format only)</t>
+  </si>
+  <si>
+    <t>cost of charity care (2010 format only)</t>
+  </si>
+  <si>
+    <t>cost of patients approved for charity care and uninsured discounts (2010 format only)</t>
   </si>
 </sst>
 </file>
@@ -752,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2BB4DF-E65D-224C-B8BB-1875153B4956}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63:F68"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1355,7 +1370,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>47</v>
@@ -1376,7 +1391,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>47</v>
@@ -1397,7 +1412,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>47</v>
@@ -1418,7 +1433,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>47</v>
@@ -1427,7 +1442,7 @@
         <v>33</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E32">
         <v>10</v>
@@ -1439,7 +1454,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>47</v>
@@ -2082,7 +2097,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>47</v>
@@ -2102,7 +2117,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>47</v>
@@ -2123,7 +2138,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>47</v>
@@ -2144,7 +2159,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>47</v>
@@ -2165,7 +2180,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>47</v>
@@ -2174,7 +2189,7 @@
         <v>56</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E68">
         <v>96</v>
@@ -2233,10 +2248,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F01AFD1-3AE8-2C43-8863-F91A96C0A348}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2251,10 +2266,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2262,10 +2277,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2273,10 +2288,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2284,10 +2299,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2295,10 +2310,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2306,7 +2321,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -2317,7 +2332,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" t="s">
         <v>85</v>
@@ -2328,7 +2343,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" t="s">
         <v>86</v>
@@ -2339,7 +2354,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
         <v>87</v>
@@ -2350,7 +2365,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
         <v>88</v>
@@ -2361,7 +2376,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C11" t="s">
         <v>89</v>
@@ -2372,7 +2387,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" t="s">
         <v>90</v>
@@ -2383,7 +2398,7 @@
         <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C13" t="s">
         <v>91</v>
@@ -2394,7 +2409,7 @@
         <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14" t="s">
         <v>92</v>
@@ -2405,7 +2420,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15" t="s">
         <v>93</v>
@@ -2416,7 +2431,7 @@
         <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" t="s">
         <v>94</v>
@@ -2427,7 +2442,7 @@
         <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
         <v>95</v>
@@ -2438,7 +2453,7 @@
         <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
         <v>96</v>
@@ -2449,7 +2464,7 @@
         <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
         <v>97</v>
@@ -2460,7 +2475,7 @@
         <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
         <v>99</v>
@@ -2471,7 +2486,7 @@
         <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C21" t="s">
         <v>100</v>
@@ -2482,10 +2497,10 @@
         <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2493,10 +2508,10 @@
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2504,7 +2519,7 @@
         <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
         <v>79</v>
@@ -2515,7 +2530,7 @@
         <v>48</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C25" t="s">
         <v>80</v>
@@ -2526,7 +2541,7 @@
         <v>49</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26" t="s">
         <v>81</v>
@@ -2537,7 +2552,7 @@
         <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
         <v>82</v>
@@ -2548,7 +2563,7 @@
         <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C28" t="s">
         <v>83</v>
@@ -2556,57 +2571,57 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2614,7 +2629,7 @@
         <v>54</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C34" t="s">
         <v>84</v>
@@ -2622,12 +2637,67 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
enable cost of charity care variable
</commit_message>
<xml_diff>
--- a/misc/lookup.xlsx
+++ b/misc/lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asacarny/Repositories/hospital-cost-reports/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2128C3-4C94-A44A-BF78-E2141C1BC4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287BBEF0-3575-3A4D-A5D4-55315B95227B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15760" yWindow="3720" windowWidth="18640" windowHeight="16120" activeTab="1" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
+    <workbookView xWindow="11600" yWindow="2380" windowWidth="18640" windowHeight="16120" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Table" sheetId="1" r:id="rId1"/>
@@ -767,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2BB4DF-E65D-224C-B8BB-1875153B4956}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:A39"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1531,7 +1531,7 @@
         <v>10</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -2250,7 +2250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F01AFD1-3AE8-2C43-8863-F91A96C0A348}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
re-enable cost of charity care variable
</commit_message>
<xml_diff>
--- a/misc/lookup.xlsx
+++ b/misc/lookup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asacarny/Repositories/hospital-cost-reports/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287BBEF0-3575-3A4D-A5D4-55315B95227B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FDB235-06AF-0446-8F32-CB168800FCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11600" yWindow="2380" windowWidth="18640" windowHeight="16120" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
   </bookViews>
@@ -767,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2BB4DF-E65D-224C-B8BB-1875153B4956}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>

</xml_diff>